<commit_message>
Aula 3 - Desenhando Mazes
* Graphs:
    - Implementado heuristica dos labirintos (distância euclidiana) para testar o A*
    - Implementado a visualização dos labirintos.
         - Podemos ver o caminho que cada heuristica passa
</commit_message>
<xml_diff>
--- a/Aula3/Mazes_aEstrela.xlsx
+++ b/Aula3/Mazes_aEstrela.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Danilo S. Tuzita\Documents\FEI\Mestrado\1.programacao-cientifica\Aula3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0187209-CFC4-4849-83CB-F0CE08365E34}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06012885-ADC0-43DE-B63D-2056648BFFEC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2704D7D-FBC1-4767-BC4B-63B86EFA04B8}"/>
   </bookViews>
@@ -311,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -342,6 +342,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82084566-17B0-4119-9909-AB32F38BC897}">
-  <dimension ref="B1:AV27"/>
+  <dimension ref="A1:AV50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AQ23" sqref="AQ23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="Y29" sqref="Y29:Y44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -669,12 +672,112 @@
     <col min="40" max="43" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+      <c r="L1">
+        <v>10</v>
+      </c>
+      <c r="M1">
+        <v>11</v>
+      </c>
+      <c r="N1">
+        <v>12</v>
+      </c>
+      <c r="O1">
+        <v>13</v>
+      </c>
+      <c r="P1">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>17</v>
+      </c>
+      <c r="T1">
+        <v>18</v>
+      </c>
+      <c r="U1">
+        <v>19</v>
+      </c>
+      <c r="V1">
+        <v>20</v>
+      </c>
+      <c r="Y1">
+        <v>0</v>
+      </c>
+      <c r="Z1">
+        <v>1</v>
+      </c>
+      <c r="AA1">
+        <v>2</v>
+      </c>
+      <c r="AB1">
+        <v>3</v>
+      </c>
+      <c r="AC1">
+        <v>4</v>
+      </c>
+      <c r="AD1">
+        <v>5</v>
+      </c>
+      <c r="AE1">
+        <v>6</v>
+      </c>
+      <c r="AF1">
+        <v>7</v>
+      </c>
+      <c r="AG1">
+        <v>8</v>
+      </c>
+      <c r="AH1">
+        <v>9</v>
+      </c>
+      <c r="AI1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="30">
         <v>1</v>
       </c>
       <c r="D2" s="3">
@@ -734,6 +837,9 @@
       <c r="V2" s="4">
         <v>0</v>
       </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
       <c r="Y2" s="2">
         <v>0</v>
       </c>
@@ -789,35 +895,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3" s="5">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="C3" s="31">
+        <v>1</v>
+      </c>
+      <c r="D3" s="31">
+        <v>1</v>
+      </c>
+      <c r="E3" s="31">
+        <v>1</v>
+      </c>
+      <c r="F3" s="31">
+        <v>1</v>
+      </c>
+      <c r="G3" s="31">
+        <v>1</v>
+      </c>
+      <c r="H3" s="31">
+        <v>1</v>
+      </c>
+      <c r="I3" s="31">
+        <v>1</v>
+      </c>
+      <c r="J3" s="31">
+        <v>1</v>
+      </c>
+      <c r="K3" s="31">
         <v>1</v>
       </c>
       <c r="L3" s="1">
@@ -829,13 +938,13 @@
       <c r="N3" s="1">
         <v>0</v>
       </c>
-      <c r="O3" s="1">
-        <v>1</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="1">
+      <c r="O3" s="31">
+        <v>1</v>
+      </c>
+      <c r="P3" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="31">
         <v>1</v>
       </c>
       <c r="R3" s="1">
@@ -853,6 +962,9 @@
       <c r="V3" s="6">
         <v>0</v>
       </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
       <c r="Y3" s="5">
         <v>0</v>
       </c>
@@ -908,7 +1020,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4" s="5">
         <v>0</v>
       </c>
@@ -936,7 +1051,7 @@
       <c r="J4" s="1">
         <v>0</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="31">
         <v>1</v>
       </c>
       <c r="L4" s="1">
@@ -948,13 +1063,13 @@
       <c r="N4" s="1">
         <v>0</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4" s="31">
         <v>1</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4" s="31">
         <v>1</v>
       </c>
       <c r="R4" s="1">
@@ -972,6 +1087,9 @@
       <c r="V4" s="6">
         <v>0</v>
       </c>
+      <c r="X4">
+        <v>2</v>
+      </c>
       <c r="Y4" s="5">
         <v>0</v>
       </c>
@@ -1027,7 +1145,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5" s="5">
         <v>0</v>
       </c>
@@ -1055,25 +1176,25 @@
       <c r="J5" s="1">
         <v>0</v>
       </c>
-      <c r="K5" s="1">
-        <v>1</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
-      <c r="M5" s="1">
-        <v>1</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1">
+      <c r="K5" s="31">
+        <v>1</v>
+      </c>
+      <c r="L5" s="31">
+        <v>1</v>
+      </c>
+      <c r="M5" s="31">
+        <v>1</v>
+      </c>
+      <c r="N5" s="31">
+        <v>1</v>
+      </c>
+      <c r="O5" s="31">
         <v>1</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="Q5" s="31">
         <v>1</v>
       </c>
       <c r="R5" s="1">
@@ -1091,6 +1212,9 @@
       <c r="V5" s="6">
         <v>0</v>
       </c>
+      <c r="X5">
+        <v>3</v>
+      </c>
       <c r="Y5" s="5">
         <v>0</v>
       </c>
@@ -1146,7 +1270,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
       <c r="B6" s="5">
         <v>0</v>
       </c>
@@ -1192,7 +1319,7 @@
       <c r="P6" s="1">
         <v>0</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="31">
         <v>1</v>
       </c>
       <c r="R6" s="1">
@@ -1209,6 +1336,9 @@
       </c>
       <c r="V6" s="6">
         <v>0</v>
+      </c>
+      <c r="X6">
+        <v>4</v>
       </c>
       <c r="Y6" s="5">
         <v>0</v>
@@ -1265,7 +1395,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
       <c r="B7" s="5">
         <v>0</v>
       </c>
@@ -1311,7 +1444,7 @@
       <c r="P7" s="1">
         <v>1</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q7" s="31">
         <v>1</v>
       </c>
       <c r="R7" s="1">
@@ -1329,6 +1462,9 @@
       <c r="V7" s="6">
         <v>0</v>
       </c>
+      <c r="X7">
+        <v>5</v>
+      </c>
       <c r="Y7" s="5">
         <v>0</v>
       </c>
@@ -1384,7 +1520,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
       <c r="B8" s="5">
         <v>0</v>
       </c>
@@ -1430,7 +1569,7 @@
       <c r="P8" s="1">
         <v>0</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="31">
         <v>1</v>
       </c>
       <c r="R8" s="1">
@@ -1448,6 +1587,9 @@
       <c r="V8" s="6">
         <v>0</v>
       </c>
+      <c r="X8">
+        <v>6</v>
+      </c>
       <c r="Y8" s="5">
         <v>0</v>
       </c>
@@ -1503,7 +1645,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9" s="5">
         <v>0</v>
       </c>
@@ -1549,13 +1694,13 @@
       <c r="P9" s="1">
         <v>1</v>
       </c>
-      <c r="Q9" s="1">
-        <v>1</v>
-      </c>
-      <c r="R9" s="1">
-        <v>1</v>
-      </c>
-      <c r="S9" s="1">
+      <c r="Q9" s="31">
+        <v>1</v>
+      </c>
+      <c r="R9" s="31">
+        <v>1</v>
+      </c>
+      <c r="S9" s="31">
         <v>1</v>
       </c>
       <c r="T9" s="1">
@@ -1567,6 +1712,9 @@
       <c r="V9" s="6">
         <v>0</v>
       </c>
+      <c r="X9">
+        <v>7</v>
+      </c>
       <c r="Y9" s="5">
         <v>0</v>
       </c>
@@ -1601,7 +1749,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
       <c r="B10" s="5">
         <v>0</v>
       </c>
@@ -1653,7 +1804,7 @@
       <c r="R10" s="1">
         <v>0</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S10" s="31">
         <v>1</v>
       </c>
       <c r="T10" s="1">
@@ -1664,6 +1815,9 @@
       </c>
       <c r="V10" s="6">
         <v>0</v>
+      </c>
+      <c r="X10">
+        <v>8</v>
       </c>
       <c r="Y10" s="5">
         <v>0</v>
@@ -1720,7 +1874,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
       <c r="B11" s="5">
         <v>0</v>
       </c>
@@ -1772,7 +1929,7 @@
       <c r="R11" s="1">
         <v>0</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11" s="31">
         <v>1</v>
       </c>
       <c r="T11" s="1">
@@ -1783,6 +1940,9 @@
       </c>
       <c r="V11" s="6">
         <v>0</v>
+      </c>
+      <c r="X11">
+        <v>9</v>
       </c>
       <c r="Y11" s="5">
         <v>0</v>
@@ -1839,7 +1999,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
       <c r="B12" s="5">
         <v>0</v>
       </c>
@@ -1891,7 +2054,7 @@
       <c r="R12" s="1">
         <v>0</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S12" s="31">
         <v>1</v>
       </c>
       <c r="T12" s="1">
@@ -1902,6 +2065,9 @@
       </c>
       <c r="V12" s="6">
         <v>0</v>
+      </c>
+      <c r="X12">
+        <v>10</v>
       </c>
       <c r="Y12" s="7">
         <v>0</v>
@@ -1958,7 +2124,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
       <c r="B13" s="5">
         <v>0</v>
       </c>
@@ -2010,7 +2179,7 @@
       <c r="R13" s="1">
         <v>0</v>
       </c>
-      <c r="S13" s="1">
+      <c r="S13" s="31">
         <v>1</v>
       </c>
       <c r="T13" s="1">
@@ -2044,7 +2213,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>12</v>
+      </c>
       <c r="B14" s="5">
         <v>0</v>
       </c>
@@ -2096,7 +2268,7 @@
       <c r="R14" s="1">
         <v>0</v>
       </c>
-      <c r="S14" s="1">
+      <c r="S14" s="31">
         <v>1</v>
       </c>
       <c r="T14" s="1">
@@ -2164,7 +2336,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="2:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
       <c r="B15" s="5">
         <v>0</v>
       </c>
@@ -2216,7 +2391,7 @@
       <c r="R15" s="1">
         <v>0</v>
       </c>
-      <c r="S15" s="1">
+      <c r="S15" s="31">
         <v>1</v>
       </c>
       <c r="T15" s="1">
@@ -2297,7 +2472,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="2:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
       <c r="B16" s="5">
         <v>0</v>
       </c>
@@ -2349,7 +2527,7 @@
       <c r="R16" s="1">
         <v>0</v>
       </c>
-      <c r="S16" s="1">
+      <c r="S16" s="31">
         <v>1</v>
       </c>
       <c r="T16" s="1">
@@ -2430,7 +2608,10 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
       <c r="B17" s="5">
         <v>0</v>
       </c>
@@ -2482,7 +2663,7 @@
       <c r="R17" s="1">
         <v>0</v>
       </c>
-      <c r="S17" s="1">
+      <c r="S17" s="31">
         <v>1</v>
       </c>
       <c r="T17" s="1">
@@ -2542,7 +2723,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
       <c r="B18" s="5">
         <v>0</v>
       </c>
@@ -2594,7 +2778,7 @@
       <c r="R18" s="1">
         <v>0</v>
       </c>
-      <c r="S18" s="1">
+      <c r="S18" s="31">
         <v>1</v>
       </c>
       <c r="T18" s="1">
@@ -2654,7 +2838,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="2:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
       <c r="B19" s="5">
         <v>0</v>
       </c>
@@ -2700,13 +2887,13 @@
       <c r="P19" s="1">
         <v>0</v>
       </c>
-      <c r="Q19" s="1">
-        <v>1</v>
-      </c>
-      <c r="R19" s="1">
-        <v>1</v>
-      </c>
-      <c r="S19" s="1">
+      <c r="Q19" s="31">
+        <v>1</v>
+      </c>
+      <c r="R19" s="31">
+        <v>1</v>
+      </c>
+      <c r="S19" s="31">
         <v>1</v>
       </c>
       <c r="T19" s="1">
@@ -2799,7 +2986,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
       <c r="B20" s="5">
         <v>0</v>
       </c>
@@ -2845,7 +3035,7 @@
       <c r="P20" s="1">
         <v>0</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="Q20" s="31">
         <v>1</v>
       </c>
       <c r="R20" s="1">
@@ -2911,7 +3101,10 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="2:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
       <c r="B21" s="5">
         <v>0</v>
       </c>
@@ -2957,19 +3150,19 @@
       <c r="P21" s="1">
         <v>0</v>
       </c>
-      <c r="Q21" s="1">
-        <v>1</v>
-      </c>
-      <c r="R21" s="1">
-        <v>1</v>
-      </c>
-      <c r="S21" s="1">
-        <v>1</v>
-      </c>
-      <c r="T21" s="1">
-        <v>1</v>
-      </c>
-      <c r="U21" s="1">
+      <c r="Q21" s="31">
+        <v>1</v>
+      </c>
+      <c r="R21" s="31">
+        <v>1</v>
+      </c>
+      <c r="S21" s="31">
+        <v>1</v>
+      </c>
+      <c r="T21" s="31">
+        <v>1</v>
+      </c>
+      <c r="U21" s="31">
         <v>1</v>
       </c>
       <c r="V21" s="6">
@@ -3023,7 +3216,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="2:48" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:48" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>20</v>
+      </c>
       <c r="B22" s="7">
         <v>0</v>
       </c>
@@ -3081,7 +3277,7 @@
       <c r="T22" s="8">
         <v>0</v>
       </c>
-      <c r="U22" s="8">
+      <c r="U22" s="32">
         <v>1</v>
       </c>
       <c r="V22" s="9">
@@ -3135,7 +3331,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="2:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="X23" s="19">
         <v>8</v>
       </c>
@@ -3184,7 +3380,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="2:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="X24" s="19">
         <v>9</v>
       </c>
@@ -3233,7 +3429,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="2:48" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:48" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" t="str">
+        <f>B2&amp;" "&amp;C2&amp;" "&amp;D2&amp;" "&amp;E2&amp;" "&amp;F2&amp;" "&amp;G2&amp;" "&amp;H2&amp;" "&amp;I2&amp;" "&amp;J2&amp;" "&amp;K2&amp;" "&amp;L2&amp;" "&amp;M2&amp;" "&amp;N2&amp;" "&amp;O2&amp;" "&amp;P2&amp;" "&amp;Q2&amp;" "&amp;R2&amp;" "&amp;S2&amp;" "&amp;T2&amp;" "&amp;U2&amp;" "&amp;V2</f>
+        <v>0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0</v>
+      </c>
       <c r="X25" s="19">
         <v>10</v>
       </c>
@@ -3282,7 +3482,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="2:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" t="str">
+        <f t="shared" ref="B26:B45" si="2">B3&amp;" "&amp;C3&amp;" "&amp;D3&amp;" "&amp;E3&amp;" "&amp;F3&amp;" "&amp;G3&amp;" "&amp;H3&amp;" "&amp;I3&amp;" "&amp;J3&amp;" "&amp;K3&amp;" "&amp;L3&amp;" "&amp;M3&amp;" "&amp;N3&amp;" "&amp;O3&amp;" "&amp;P3&amp;" "&amp;Q3&amp;" "&amp;R3&amp;" "&amp;S3&amp;" "&amp;T3&amp;" "&amp;U3&amp;" "&amp;V3</f>
+        <v>0 1 1 1 1 1 1 1 1 1 1 1 0 1 1 1 0 1 1 1 0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 0 0 0 0 0 0 0 1 0 0 0 1 0 1 0 0 0 1 0</v>
+      </c>
       <c r="Y27">
         <v>1</v>
       </c>
@@ -3339,6 +3549,190 @@
       </c>
       <c r="AQ27">
         <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 1 1 0 1 0 1 0 1 1 1 1 1 0 1 0 1 1 1 0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" t="str">
+        <f t="shared" si="2"/>
+        <v>0 0 0 1 0 1 0 1 0 1 0 0 0 0 0 1 0 0 0 1 0</v>
+      </c>
+      <c r="Y29" t="str">
+        <f>Y2&amp;" "&amp;Z2&amp;" "&amp;AA2&amp;" "&amp;AB2&amp;" "&amp;AC2&amp;" "&amp;AD2&amp;" "&amp;AE2&amp;" "&amp;AF2&amp;" "&amp;AG2&amp;" "&amp;AH2&amp;" "&amp;AI2</f>
+        <v>0 1 0 1 1 1 0 0 0 0 0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 0 1 0 1 1 1 1 1 1 1 0 1 1 1 1 1 1 1 0</v>
+      </c>
+      <c r="Y30" t="str">
+        <f t="shared" ref="Y30:Y40" si="3">Y3&amp;" "&amp;Z3&amp;" "&amp;AA3&amp;" "&amp;AB3&amp;" "&amp;AC3&amp;" "&amp;AD3&amp;" "&amp;AE3&amp;" "&amp;AF3&amp;" "&amp;AG3&amp;" "&amp;AH3&amp;" "&amp;AI3</f>
+        <v>0 1 1 1 0 1 1 1 1 1 0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 0 0 0 1 0 1 0 1 0 0 0 0 0 1 0 0 0 1 0</v>
+      </c>
+      <c r="Y31" t="str">
+        <f t="shared" si="3"/>
+        <v>0 0 0 1 0 1 0 0 0 1 0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 1 1 1 1 0 1 0 1 0 1 1 1 1 1 1 1 0 1 0</v>
+      </c>
+      <c r="Y32" t="str">
+        <f t="shared" si="3"/>
+        <v>0 1 1 1 0 1 0 1 0 1 0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" t="str">
+        <f t="shared" si="2"/>
+        <v>0 0 0 0 0 1 0 0 0 0 0 1 0 0 0 1 0 1 0 0 0</v>
+      </c>
+      <c r="Y33" t="str">
+        <f t="shared" si="3"/>
+        <v>0 1 0 5 0 1 0 1 0 1 0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 1 1 0 1 1 1 0 1 1 1 0 1 1 1 0 1 1 1 0</v>
+      </c>
+      <c r="Y34" t="str">
+        <f t="shared" si="3"/>
+        <v>0 1 1 1 1 1 0 1 1 1 0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" t="str">
+        <f t="shared" si="2"/>
+        <v>0 0 0 1 0 0 0 1 0 0 0 1 0 1 0 0 0 1 0 0 0</v>
+      </c>
+      <c r="Y35" t="str">
+        <f t="shared" si="3"/>
+        <v>0 1 0 0 0 1 0 0 0 1 0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 1 1 1 1 1 1 0 1 1 1 0 1 1 1 0 1 0 1 0</v>
+      </c>
+      <c r="Y36" t="str">
+        <f t="shared" si="3"/>
+        <v>0 1 0 1 0 1 1 1 0 1 0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 0 0 0 0 0 1 0 0 0 0 0 0 0 1 0 1 0 1 0</v>
+      </c>
+      <c r="Y37" t="str">
+        <f t="shared" si="3"/>
+        <v>0 0 0 1 0 0 0 1 0 1 0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 1 1 0 1 0 1 1 1 0 1 0 1 0 1 0 1 1 1 0</v>
+      </c>
+      <c r="Y38" t="str">
+        <f t="shared" si="3"/>
+        <v>0 1 1 1 1 1 1 1 1 1 0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 0 1 0 1 0 0 0 1 0 1 0 1 0 0 0 1 0 1 0</v>
+      </c>
+      <c r="Y39" t="str">
+        <f t="shared" si="3"/>
+        <v>0 0 0 0 0 0 0 0 0 1 0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 0 1 0 1 1 1 1 1 1 1 0 1 1 1 0 1 0 1 0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" t="str">
+        <f t="shared" si="2"/>
+        <v>0 0 0 1 0 0 0 0 0 0 0 0 0 1 0 1 0 1 0 0 0</v>
+      </c>
+      <c r="Y41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 0 1 1 1 0 1 0 1 0 1 1 1 0 1 1 1 0 1 0</v>
+      </c>
+      <c r="Y42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 0 1 0 0 0 1 0 1 0 0 0 1 0 1 0 0 0 1 0</v>
+      </c>
+      <c r="Y43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" t="str">
+        <f t="shared" si="2"/>
+        <v>0 1 1 1 0 1 1 1 1 1 1 1 1 1 0 1 1 1 1 1 0</v>
+      </c>
+      <c r="Y44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" t="str">
+        <f t="shared" si="2"/>
+        <v>0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>